<commit_message>
Update importer_spec tests and import test xls file.
</commit_message>
<xml_diff>
--- a/spec/fixtures/files/baddata2015test.xlsx
+++ b/spec/fixtures/files/baddata2015test.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26915"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27224"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mmo/Library/Mobile Documents/com~apple~CloudDocs/OpenSplitTime/Test Data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mark/Development/OpenSplitTime/spec/fixtures/files/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -541,7 +541,7 @@
   <dimension ref="A1:O15"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="K3" sqref="K3"/>
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -829,7 +829,7 @@
         <v>30</v>
       </c>
       <c r="H7" s="1">
-        <v>0</v>
+        <v>2.0833333333333332E-2</v>
       </c>
       <c r="I7" s="1">
         <v>0.11944444444444445</v>
@@ -1100,7 +1100,7 @@
         <v>135</v>
       </c>
       <c r="H13" s="1">
-        <v>0</v>
+        <v>4.1666666666666664E-2</v>
       </c>
       <c r="I13" s="1">
         <v>0.12847222222222224</v>

</xml_diff>

<commit_message>
Refactor EffortImporter; eliminate split_time creation for DNS effort; tweak importer_spec tests and test spreadsheet.
</commit_message>
<xml_diff>
--- a/spec/fixtures/files/baddata2015test.xlsx
+++ b/spec/fixtures/files/baddata2015test.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27224"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27610"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="64">
   <si>
     <t>first_name</t>
   </si>
@@ -119,12 +119,6 @@
     <t>Indonesia</t>
   </si>
   <si>
-    <t>Bavaria</t>
-  </si>
-  <si>
-    <t>Champagne</t>
-  </si>
-  <si>
     <t>tx</t>
   </si>
   <si>
@@ -134,12 +128,6 @@
     <t>Surrey</t>
   </si>
   <si>
-    <t>Westchester</t>
-  </si>
-  <si>
-    <t>London</t>
-  </si>
-  <si>
     <t>Ulster</t>
   </si>
   <si>
@@ -170,12 +158,6 @@
     <t>Female</t>
   </si>
   <si>
-    <t>Got</t>
-  </si>
-  <si>
-    <t>Chicked</t>
-  </si>
-  <si>
     <t>Another</t>
   </si>
   <si>
@@ -191,9 +173,6 @@
     <t>NoFirstName</t>
   </si>
   <si>
-    <t>A Frenchy</t>
-  </si>
-  <si>
     <t>French-Dude</t>
   </si>
   <si>
@@ -213,6 +192,36 @@
   </si>
   <si>
     <t>Riverdance</t>
+  </si>
+  <si>
+    <t>Hamburg</t>
+  </si>
+  <si>
+    <t>centre</t>
+  </si>
+  <si>
+    <t>Buckinghamshire</t>
+  </si>
+  <si>
+    <t>Liverpool</t>
+  </si>
+  <si>
+    <t>Hyphenated</t>
+  </si>
+  <si>
+    <t>Michael</t>
+  </si>
+  <si>
+    <t>Baldwin</t>
+  </si>
+  <si>
+    <t>Male</t>
+  </si>
+  <si>
+    <t>FEM</t>
+  </si>
+  <si>
+    <t>male</t>
   </si>
 </sst>
 </file>
@@ -541,7 +550,7 @@
   <dimension ref="A1:O15"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -578,7 +587,7 @@
         <v>16</v>
       </c>
       <c r="K1" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="L1" t="s">
         <v>17</v>
@@ -624,16 +633,16 @@
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="B3" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="C3" t="s">
         <v>7</v>
       </c>
       <c r="D3" t="s">
-        <v>29</v>
+        <v>54</v>
       </c>
       <c r="E3" t="s">
         <v>21</v>
@@ -671,16 +680,16 @@
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="B4" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="C4" t="s">
-        <v>7</v>
+        <v>61</v>
       </c>
       <c r="D4" t="s">
-        <v>30</v>
+        <v>55</v>
       </c>
       <c r="E4" t="s">
         <v>22</v>
@@ -718,16 +727,16 @@
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="B5" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="C5" t="s">
         <v>7</v>
       </c>
       <c r="D5" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E5" t="s">
         <v>23</v>
@@ -761,16 +770,16 @@
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="B6" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="C6" t="s">
         <v>10</v>
       </c>
       <c r="D6" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="E6" t="s">
         <v>8</v>
@@ -808,16 +817,16 @@
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>46</v>
+        <v>59</v>
       </c>
       <c r="B7" t="s">
-        <v>47</v>
+        <v>60</v>
       </c>
       <c r="C7" t="s">
         <v>7</v>
       </c>
       <c r="D7" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="E7" t="s">
         <v>24</v>
@@ -855,16 +864,16 @@
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="B8" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="C8" t="s">
         <v>7</v>
       </c>
       <c r="D8" t="s">
-        <v>34</v>
+        <v>56</v>
       </c>
       <c r="E8" t="s">
         <v>25</v>
@@ -902,16 +911,16 @@
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="B9" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="C9" t="s">
-        <v>10</v>
+        <v>62</v>
       </c>
       <c r="D9" t="s">
-        <v>35</v>
+        <v>57</v>
       </c>
       <c r="E9" t="s">
         <v>26</v>
@@ -949,13 +958,13 @@
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="C10" t="s">
         <v>7</v>
       </c>
       <c r="D10" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="E10" t="s">
         <v>27</v>
@@ -991,13 +1000,13 @@
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B11" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="C11" t="s">
         <v>7</v>
       </c>
       <c r="D11" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="E11" t="s">
         <v>28</v>
@@ -1035,16 +1044,16 @@
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="B12" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="C12" t="s">
         <v>7</v>
       </c>
       <c r="D12" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="E12" t="s">
         <v>11</v>
@@ -1079,13 +1088,13 @@
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="B13" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="C13" t="s">
-        <v>7</v>
+        <v>63</v>
       </c>
       <c r="D13" t="s">
         <v>9</v>
@@ -1132,10 +1141,10 @@
         <v>7</v>
       </c>
       <c r="D14" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="E14" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="F14">
         <v>58</v>
@@ -1176,7 +1185,7 @@
         <v>10</v>
       </c>
       <c r="D15" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="E15" t="s">
         <v>8</v>

</xml_diff>

<commit_message>
Modify EffortImportDataPreparer to handle age parameter == 0; streamline importer_spec and add test cases for age == 0; update effort spec; expand EffortImportDataPreparer spec with tests for age parameter; update test spreadsheet file; define basic factories for course, event, effort, and participant.
</commit_message>
<xml_diff>
--- a/spec/fixtures/files/baddata2015test.xlsx
+++ b/spec/fixtures/files/baddata2015test.xlsx
@@ -15,7 +15,7 @@
     <sheet name="hardrock2015" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">hardrock2015!$A$1:$J$6</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">hardrock2015!$A$1:$K$6</definedName>
   </definedNames>
   <calcPr calcId="0" concurrentCalc="0"/>
   <extLst>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="65">
   <si>
     <t>first_name</t>
   </si>
@@ -222,6 +222,9 @@
   </si>
   <si>
     <t>male</t>
+  </si>
+  <si>
+    <t>birthdate</t>
   </si>
 </sst>
 </file>
@@ -263,10 +266,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="46" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -547,15 +551,15 @@
   <sheetPr enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:O15"/>
+  <dimension ref="A1:P15"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -575,63 +579,66 @@
         <v>12</v>
       </c>
       <c r="G1" t="s">
+        <v>64</v>
+      </c>
+      <c r="H1" t="s">
         <v>4</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>5</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>15</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>16</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>53</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>17</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>18</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>19</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>14</v>
       </c>
-      <c r="H2">
+      <c r="I2">
         <v>0</v>
-      </c>
-      <c r="I2">
-        <v>6.5</v>
       </c>
       <c r="J2">
         <v>6.5</v>
       </c>
       <c r="K2">
+        <v>6.5</v>
+      </c>
+      <c r="L2">
         <v>33</v>
       </c>
-      <c r="L2">
+      <c r="M2">
         <v>40</v>
-      </c>
-      <c r="M2">
-        <v>46.6</v>
       </c>
       <c r="N2">
         <v>46.6</v>
       </c>
       <c r="O2">
+        <v>46.6</v>
+      </c>
+      <c r="P2">
         <v>51.3</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>38</v>
       </c>
@@ -650,35 +657,38 @@
       <c r="F3">
         <v>28</v>
       </c>
-      <c r="G3">
+      <c r="G3" s="3">
+        <v>31809</v>
+      </c>
+      <c r="H3">
         <v>1</v>
       </c>
-      <c r="H3" s="1">
+      <c r="I3" s="1">
         <v>0</v>
-      </c>
-      <c r="I3" s="1">
-        <v>7.8472222222222221E-2</v>
       </c>
       <c r="J3" s="1">
         <v>7.8472222222222221E-2</v>
       </c>
       <c r="K3" s="1">
+        <v>7.8472222222222221E-2</v>
+      </c>
+      <c r="L3" s="1">
         <v>0.5625</v>
       </c>
-      <c r="L3" s="1">
+      <c r="M3" s="1">
         <v>0.8652777777777777</v>
-      </c>
-      <c r="M3" s="1">
-        <v>0.93125000000000002</v>
       </c>
       <c r="N3" s="1">
         <v>0.93125000000000002</v>
       </c>
       <c r="O3" s="1">
+        <v>0.93125000000000002</v>
+      </c>
+      <c r="P3" s="1">
         <v>0.97777777777777775</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>52</v>
       </c>
@@ -697,35 +707,38 @@
       <c r="F4">
         <v>32</v>
       </c>
-      <c r="G4">
+      <c r="G4" s="3">
+        <v>30390</v>
+      </c>
+      <c r="H4">
         <v>128</v>
       </c>
-      <c r="H4" s="1">
+      <c r="I4" s="1">
         <v>0</v>
-      </c>
-      <c r="I4" s="1">
-        <v>8.4027777777777771E-2</v>
       </c>
       <c r="J4" s="1">
         <v>8.4027777777777771E-2</v>
       </c>
       <c r="K4" s="1">
+        <v>8.4027777777777771E-2</v>
+      </c>
+      <c r="L4" s="1">
         <v>0.58402777777777781</v>
       </c>
-      <c r="L4" s="1">
+      <c r="M4" s="1">
         <v>0.94791666666666663</v>
-      </c>
-      <c r="M4" s="2">
-        <v>0.84861111111111109</v>
       </c>
       <c r="N4" s="2">
         <v>0.84861111111111109</v>
       </c>
       <c r="O4" s="2">
+        <v>0.84861111111111109</v>
+      </c>
+      <c r="P4" s="2">
         <v>1.0729166666666667</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>50</v>
       </c>
@@ -744,31 +757,31 @@
       <c r="F5">
         <v>36</v>
       </c>
-      <c r="G5">
+      <c r="H5">
         <v>2</v>
       </c>
-      <c r="H5" s="1">
+      <c r="I5" s="1">
         <v>0</v>
       </c>
-      <c r="I5" s="1">
+      <c r="J5" s="1">
         <v>7.8472222222222221E-2</v>
       </c>
-      <c r="J5" s="1"/>
       <c r="K5" s="1"/>
-      <c r="L5" s="1">
+      <c r="L5" s="1"/>
+      <c r="M5" s="1">
         <v>0.97361111111111109</v>
       </c>
-      <c r="M5" s="2">
+      <c r="N5" s="2">
         <v>1.0631944444444443</v>
       </c>
-      <c r="N5" s="2">
+      <c r="O5" s="2">
         <v>1.0638888888888889</v>
       </c>
-      <c r="O5" s="2">
+      <c r="P5" s="2">
         <v>1.117361111111111</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>40</v>
       </c>
@@ -785,37 +798,37 @@
         <v>8</v>
       </c>
       <c r="F6">
-        <v>42</v>
-      </c>
-      <c r="G6">
+        <v>25</v>
+      </c>
+      <c r="H6">
         <v>143</v>
       </c>
-      <c r="H6" s="1">
+      <c r="I6" s="1">
         <v>0</v>
-      </c>
-      <c r="I6" s="1">
-        <v>8.4027777777777771E-2</v>
       </c>
       <c r="J6" s="1">
         <v>8.4027777777777771E-2</v>
       </c>
       <c r="K6" s="1">
+        <v>8.4027777777777771E-2</v>
+      </c>
+      <c r="L6" s="1">
         <v>0.59722222222222221</v>
       </c>
-      <c r="L6" s="1">
+      <c r="M6" s="1">
         <v>0.98541666666666661</v>
       </c>
-      <c r="M6" s="2">
+      <c r="N6" s="2">
         <v>1.0763888888888888</v>
       </c>
-      <c r="N6" s="2">
+      <c r="O6" s="2">
         <v>1.0770833333333334</v>
       </c>
-      <c r="O6" s="2">
+      <c r="P6" s="2">
         <v>1.1270833333333334</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>59</v>
       </c>
@@ -832,37 +845,37 @@
         <v>24</v>
       </c>
       <c r="F7">
-        <v>54</v>
-      </c>
-      <c r="G7">
+        <v>51</v>
+      </c>
+      <c r="H7">
         <v>30</v>
       </c>
-      <c r="H7" s="1">
+      <c r="I7" s="1">
         <v>2.0833333333333332E-2</v>
-      </c>
-      <c r="I7" s="1">
-        <v>0.11944444444444445</v>
       </c>
       <c r="J7" s="1">
         <v>0.11944444444444445</v>
       </c>
-      <c r="K7" s="2">
+      <c r="K7" s="1">
+        <v>0.11944444444444445</v>
+      </c>
+      <c r="L7" s="2">
         <v>0.84722222222222221</v>
       </c>
-      <c r="L7" s="2">
+      <c r="M7" s="2">
         <v>1.5625</v>
       </c>
-      <c r="M7" s="2">
+      <c r="N7" s="2">
         <v>1.7236111111111112</v>
       </c>
-      <c r="N7" s="2">
+      <c r="O7" s="2">
         <v>1.73125</v>
       </c>
-      <c r="O7" s="2">
+      <c r="P7" s="2">
         <v>1.8305555555555555</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>42</v>
       </c>
@@ -881,35 +894,35 @@
       <c r="F8">
         <v>41</v>
       </c>
-      <c r="G8">
+      <c r="H8">
         <v>186</v>
       </c>
-      <c r="H8" s="1">
+      <c r="I8" s="1">
         <v>0</v>
-      </c>
-      <c r="I8" s="1">
-        <v>0.11805555555555557</v>
       </c>
       <c r="J8" s="1">
         <v>0.11805555555555557</v>
       </c>
-      <c r="K8" s="2">
+      <c r="K8" s="1">
+        <v>0.11805555555555557</v>
+      </c>
+      <c r="L8" s="2">
         <v>0.94027777777777777</v>
       </c>
-      <c r="L8" s="2">
+      <c r="M8" s="2">
         <v>1.5729166666666667</v>
       </c>
-      <c r="M8" s="2">
+      <c r="N8" s="2">
         <v>1.7229166666666667</v>
       </c>
-      <c r="N8" s="2">
+      <c r="O8" s="2">
         <v>1.7249999999999999</v>
       </c>
-      <c r="O8" s="2">
+      <c r="P8" s="2">
         <v>1.8319444444444446</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>44</v>
       </c>
@@ -928,35 +941,35 @@
       <c r="F9">
         <v>45</v>
       </c>
-      <c r="G9">
+      <c r="H9">
         <v>40</v>
       </c>
-      <c r="H9" s="1">
+      <c r="I9" s="1">
         <v>0</v>
-      </c>
-      <c r="I9" s="1">
-        <v>0.12916666666666668</v>
       </c>
       <c r="J9" s="1">
         <v>0.12916666666666668</v>
       </c>
-      <c r="K9" s="2">
+      <c r="K9" s="1">
+        <v>0.12916666666666668</v>
+      </c>
+      <c r="L9" s="2">
         <v>1.0347222222222221</v>
       </c>
-      <c r="L9" s="2">
+      <c r="M9" s="2">
         <v>1.6319444444444444</v>
       </c>
-      <c r="M9" s="2">
+      <c r="N9" s="2">
         <v>1.7944444444444445</v>
       </c>
-      <c r="N9" s="2">
+      <c r="O9" s="2">
         <v>1.7958333333333334</v>
       </c>
-      <c r="O9" s="2">
+      <c r="P9" s="2">
         <v>1.8965277777777778</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>45</v>
       </c>
@@ -972,33 +985,33 @@
       <c r="F10">
         <v>50</v>
       </c>
-      <c r="G10">
+      <c r="H10">
         <v>131</v>
       </c>
-      <c r="H10" s="1">
+      <c r="I10" s="1">
         <v>0</v>
-      </c>
-      <c r="I10" s="1">
-        <v>0.12847222222222224</v>
       </c>
       <c r="J10" s="1">
         <v>0.12847222222222224</v>
       </c>
-      <c r="K10" s="2">
+      <c r="K10" s="1">
+        <v>0.12847222222222224</v>
+      </c>
+      <c r="L10" s="2">
         <v>1.0374999999999999</v>
       </c>
-      <c r="L10" s="2"/>
-      <c r="M10" s="2">
+      <c r="M10" s="2"/>
+      <c r="N10" s="2">
         <v>1.8090277777777777</v>
       </c>
-      <c r="N10" s="2">
+      <c r="O10" s="2">
         <v>1.8138888888888889</v>
       </c>
-      <c r="O10" s="2">
+      <c r="P10" s="2">
         <v>1.9048611111111111</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B11" t="s">
         <v>46</v>
       </c>
@@ -1014,35 +1027,35 @@
       <c r="F11">
         <v>41</v>
       </c>
-      <c r="G11">
+      <c r="H11">
         <v>122</v>
       </c>
-      <c r="H11" s="1">
+      <c r="I11" s="1">
         <v>0</v>
-      </c>
-      <c r="I11" s="1">
-        <v>0.12847222222222224</v>
       </c>
       <c r="J11" s="1">
         <v>0.12847222222222224</v>
       </c>
-      <c r="K11" s="2">
+      <c r="K11" s="1">
+        <v>0.12847222222222224</v>
+      </c>
+      <c r="L11" s="2">
         <v>0.91736111111111107</v>
       </c>
-      <c r="L11" s="2">
+      <c r="M11" s="2">
         <v>1.7388888888888889</v>
       </c>
-      <c r="M11" s="2">
+      <c r="N11" s="2">
         <v>1.9152777777777779</v>
       </c>
-      <c r="N11" s="2">
+      <c r="O11" s="2">
         <v>1.9166666666666667</v>
       </c>
-      <c r="O11" s="2">
+      <c r="P11" s="2">
         <v>1.9993055555555557</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>58</v>
       </c>
@@ -1061,32 +1074,32 @@
       <c r="F12">
         <v>62</v>
       </c>
-      <c r="G12">
+      <c r="H12">
         <v>49</v>
       </c>
-      <c r="H12" s="1">
+      <c r="I12" s="1">
         <v>0</v>
-      </c>
-      <c r="I12" s="1">
-        <v>0.11666666666666665</v>
       </c>
       <c r="J12" s="1">
         <v>0.11666666666666665</v>
       </c>
-      <c r="K12" s="2">
+      <c r="K12" s="1">
+        <v>0.11666666666666665</v>
+      </c>
+      <c r="L12" s="2">
         <v>1.2527777777777778</v>
       </c>
-      <c r="L12" s="2">
+      <c r="M12" s="2">
         <v>1.7222222222222223</v>
-      </c>
-      <c r="M12" s="2">
-        <v>1.8993055555555556</v>
       </c>
       <c r="N12" s="2">
         <v>1.8993055555555556</v>
       </c>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="O12" s="2">
+        <v>1.8993055555555556</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>48</v>
       </c>
@@ -1103,34 +1116,34 @@
         <v>8</v>
       </c>
       <c r="F13">
-        <v>51</v>
-      </c>
-      <c r="G13">
+        <v>0</v>
+      </c>
+      <c r="H13">
         <v>135</v>
       </c>
-      <c r="H13" s="1">
+      <c r="I13" s="1">
         <v>4.1666666666666664E-2</v>
-      </c>
-      <c r="I13" s="1">
-        <v>0.12847222222222224</v>
       </c>
       <c r="J13" s="1">
         <v>0.12847222222222224</v>
       </c>
-      <c r="K13" s="2">
+      <c r="K13" s="1">
+        <v>0.12847222222222224</v>
+      </c>
+      <c r="L13" s="2">
         <v>1.1805555555555556</v>
       </c>
-      <c r="L13" s="2">
+      <c r="M13" s="2">
         <v>1.8041666666666665</v>
-      </c>
-      <c r="M13" s="2">
-        <v>1.95</v>
       </c>
       <c r="N13" s="2">
         <v>1.95</v>
       </c>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="O13" s="2">
+        <v>1.95</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>20</v>
       </c>
@@ -1146,35 +1159,32 @@
       <c r="E14" t="s">
         <v>34</v>
       </c>
-      <c r="F14">
-        <v>58</v>
-      </c>
-      <c r="G14">
+      <c r="H14">
         <v>32</v>
       </c>
-      <c r="H14" s="1">
+      <c r="I14" s="1">
         <v>0</v>
-      </c>
-      <c r="I14" s="1">
-        <v>0.12847222222222224</v>
       </c>
       <c r="J14" s="1">
         <v>0.12847222222222224</v>
       </c>
-      <c r="K14" s="2">
+      <c r="K14" s="1">
+        <v>0.12847222222222224</v>
+      </c>
+      <c r="L14" s="2">
         <v>1.3472222222222223</v>
       </c>
-      <c r="L14" s="2">
+      <c r="M14" s="2">
         <v>1.7562499999999999</v>
       </c>
-      <c r="M14" s="2">
+      <c r="N14" s="2">
         <v>1.9284722222222221</v>
       </c>
-      <c r="N14" s="2">
+      <c r="O14" s="2">
         <v>1.9291666666666665</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>20</v>
       </c>
@@ -1193,12 +1203,12 @@
       <c r="F15">
         <v>49</v>
       </c>
-      <c r="G15">
+      <c r="H15">
         <v>119</v>
       </c>
-      <c r="H15" s="1"/>
       <c r="I15" s="1"/>
       <c r="J15" s="1"/>
+      <c r="K15" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>

<commit_message>
Finish EffortSplitTimeCreator service and add spec; remove unnecessary code from BulkUpdateService::bulk_update_start_offset; expand basic factory test framework; update test spreadsheet file; further streamline importer_spec.
</commit_message>
<xml_diff>
--- a/spec/fixtures/files/baddata2015test.xlsx
+++ b/spec/fixtures/files/baddata2015test.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mark/Development/OpenSplitTime/spec/fixtures/files/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mmo/Development/OpenSplitTime/spec/fixtures/files/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17460" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25300" windowHeight="18900" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="hardrock2015" sheetId="1" r:id="rId1"/>
@@ -246,12 +246,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -266,11 +272,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="46" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="20" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="46" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="15" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -554,10 +564,15 @@
   <dimension ref="A1:P15"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="M6" sqref="M6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="10" max="10" width="10.83203125" style="4"/>
+    <col min="13" max="13" width="10.83203125" style="4"/>
+    <col min="15" max="16" width="10.83203125" style="4"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
@@ -587,7 +602,7 @@
       <c r="I1" t="s">
         <v>5</v>
       </c>
-      <c r="J1" t="s">
+      <c r="J1" s="4" t="s">
         <v>15</v>
       </c>
       <c r="K1" t="s">
@@ -596,16 +611,16 @@
       <c r="L1" t="s">
         <v>53</v>
       </c>
-      <c r="M1" t="s">
+      <c r="M1" s="4" t="s">
         <v>17</v>
       </c>
       <c r="N1" t="s">
         <v>18</v>
       </c>
-      <c r="O1" t="s">
+      <c r="O1" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="P1" t="s">
+      <c r="P1" s="4" t="s">
         <v>6</v>
       </c>
     </row>
@@ -616,7 +631,7 @@
       <c r="I2">
         <v>0</v>
       </c>
-      <c r="J2">
+      <c r="J2" s="4">
         <v>6.5</v>
       </c>
       <c r="K2">
@@ -625,16 +640,16 @@
       <c r="L2">
         <v>33</v>
       </c>
-      <c r="M2">
+      <c r="M2" s="4">
         <v>40</v>
       </c>
       <c r="N2">
         <v>46.6</v>
       </c>
-      <c r="O2">
+      <c r="O2" s="4">
         <v>46.6</v>
       </c>
-      <c r="P2">
+      <c r="P2" s="4">
         <v>51.3</v>
       </c>
     </row>
@@ -666,7 +681,7 @@
       <c r="I3" s="1">
         <v>0</v>
       </c>
-      <c r="J3" s="1">
+      <c r="J3" s="5">
         <v>7.8472222222222221E-2</v>
       </c>
       <c r="K3" s="1">
@@ -675,66 +690,66 @@
       <c r="L3" s="1">
         <v>0.5625</v>
       </c>
-      <c r="M3" s="1">
+      <c r="M3" s="5">
         <v>0.8652777777777777</v>
       </c>
       <c r="N3" s="1">
         <v>0.93125000000000002</v>
       </c>
-      <c r="O3" s="1">
+      <c r="O3" s="5">
         <v>0.93125000000000002</v>
       </c>
-      <c r="P3" s="1">
+      <c r="P3" s="5">
         <v>0.97777777777777775</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+    <row r="4" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="F4">
+      <c r="F4" s="4">
         <v>32</v>
       </c>
-      <c r="G4" s="3">
+      <c r="G4" s="7">
         <v>30390</v>
       </c>
-      <c r="H4">
+      <c r="H4" s="4">
         <v>128</v>
       </c>
-      <c r="I4" s="1">
+      <c r="I4" s="5">
         <v>0</v>
       </c>
-      <c r="J4" s="1">
+      <c r="J4" s="5">
         <v>8.4027777777777771E-2</v>
       </c>
-      <c r="K4" s="1">
+      <c r="K4" s="5">
         <v>8.4027777777777771E-2</v>
       </c>
-      <c r="L4" s="1">
+      <c r="L4" s="5">
         <v>0.58402777777777781</v>
       </c>
-      <c r="M4" s="1">
+      <c r="M4" s="5">
         <v>0.94791666666666663</v>
       </c>
-      <c r="N4" s="2">
+      <c r="N4" s="6">
         <v>0.84861111111111109</v>
       </c>
-      <c r="O4" s="2">
+      <c r="O4" s="6">
         <v>0.84861111111111109</v>
       </c>
-      <c r="P4" s="2">
+      <c r="P4" s="6">
         <v>1.0729166666666667</v>
       </c>
     </row>
@@ -763,68 +778,68 @@
       <c r="I5" s="1">
         <v>0</v>
       </c>
-      <c r="J5" s="1">
+      <c r="J5" s="5">
         <v>7.8472222222222221E-2</v>
       </c>
       <c r="K5" s="1"/>
       <c r="L5" s="1"/>
-      <c r="M5" s="1">
+      <c r="M5" s="5">
         <v>0.97361111111111109</v>
       </c>
       <c r="N5" s="2">
         <v>1.0631944444444443</v>
       </c>
-      <c r="O5" s="2">
+      <c r="O5" s="6">
         <v>1.0638888888888889</v>
       </c>
-      <c r="P5" s="2">
+      <c r="P5" s="6">
         <v>1.117361111111111</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
+    <row r="6" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E6" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="F6">
+      <c r="F6" s="4">
         <v>25</v>
       </c>
-      <c r="H6">
+      <c r="H6" s="4">
         <v>143</v>
       </c>
-      <c r="I6" s="1">
+      <c r="I6" s="5">
         <v>0</v>
       </c>
-      <c r="J6" s="1">
+      <c r="J6" s="5">
+        <v>9.0277777777777776E-2</v>
+      </c>
+      <c r="K6" s="5">
         <v>8.4027777777777771E-2</v>
       </c>
-      <c r="K6" s="1">
-        <v>8.4027777777777771E-2</v>
-      </c>
-      <c r="L6" s="1">
+      <c r="L6" s="5">
         <v>0.59722222222222221</v>
       </c>
-      <c r="M6" s="1">
+      <c r="M6" s="5">
         <v>0.98541666666666661</v>
       </c>
-      <c r="N6" s="2">
+      <c r="N6" s="6">
         <v>1.0763888888888888</v>
       </c>
-      <c r="O6" s="2">
+      <c r="O6" s="6">
         <v>1.0770833333333334</v>
       </c>
-      <c r="P6" s="2">
+      <c r="P6" s="6">
         <v>1.1270833333333334</v>
       </c>
     </row>
@@ -853,7 +868,7 @@
       <c r="I7" s="1">
         <v>2.0833333333333332E-2</v>
       </c>
-      <c r="J7" s="1">
+      <c r="J7" s="5">
         <v>0.11944444444444445</v>
       </c>
       <c r="K7" s="1">
@@ -862,63 +877,63 @@
       <c r="L7" s="2">
         <v>0.84722222222222221</v>
       </c>
-      <c r="M7" s="2">
+      <c r="M7" s="6">
         <v>1.5625</v>
       </c>
       <c r="N7" s="2">
         <v>1.7236111111111112</v>
       </c>
-      <c r="O7" s="2">
+      <c r="O7" s="6">
         <v>1.73125</v>
       </c>
-      <c r="P7" s="2">
+      <c r="P7" s="6">
         <v>1.8305555555555555</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
+    <row r="8" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D8" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="E8" t="s">
+      <c r="E8" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="F8">
+      <c r="F8" s="4">
         <v>41</v>
       </c>
-      <c r="H8">
+      <c r="H8" s="4">
         <v>186</v>
       </c>
-      <c r="I8" s="1">
+      <c r="I8" s="5">
         <v>0</v>
       </c>
-      <c r="J8" s="1">
+      <c r="J8" s="5">
         <v>0.11805555555555557</v>
       </c>
-      <c r="K8" s="1">
+      <c r="K8" s="5">
         <v>0.11805555555555557</v>
       </c>
-      <c r="L8" s="2">
+      <c r="L8" s="6">
         <v>0.94027777777777777</v>
       </c>
-      <c r="M8" s="2">
+      <c r="M8" s="6">
         <v>1.5729166666666667</v>
       </c>
-      <c r="N8" s="2">
+      <c r="N8" s="6">
         <v>1.7229166666666667</v>
       </c>
-      <c r="O8" s="2">
+      <c r="O8" s="6">
         <v>1.7249999999999999</v>
       </c>
-      <c r="P8" s="2">
+      <c r="P8" s="6">
         <v>1.8319444444444446</v>
       </c>
     </row>
@@ -947,7 +962,7 @@
       <c r="I9" s="1">
         <v>0</v>
       </c>
-      <c r="J9" s="1">
+      <c r="J9" s="5">
         <v>0.12916666666666668</v>
       </c>
       <c r="K9" s="1">
@@ -956,16 +971,16 @@
       <c r="L9" s="2">
         <v>1.0347222222222221</v>
       </c>
-      <c r="M9" s="2">
+      <c r="M9" s="6">
         <v>1.6319444444444444</v>
       </c>
       <c r="N9" s="2">
         <v>1.7944444444444445</v>
       </c>
-      <c r="O9" s="2">
+      <c r="O9" s="6">
         <v>1.7958333333333334</v>
       </c>
-      <c r="P9" s="2">
+      <c r="P9" s="6">
         <v>1.8965277777777778</v>
       </c>
     </row>
@@ -991,7 +1006,7 @@
       <c r="I10" s="1">
         <v>0</v>
       </c>
-      <c r="J10" s="1">
+      <c r="J10" s="5">
         <v>0.12847222222222224</v>
       </c>
       <c r="K10" s="1">
@@ -1000,14 +1015,14 @@
       <c r="L10" s="2">
         <v>1.0374999999999999</v>
       </c>
-      <c r="M10" s="2"/>
+      <c r="M10" s="6"/>
       <c r="N10" s="2">
         <v>1.8090277777777777</v>
       </c>
-      <c r="O10" s="2">
+      <c r="O10" s="6">
         <v>1.8138888888888889</v>
       </c>
-      <c r="P10" s="2">
+      <c r="P10" s="6">
         <v>1.9048611111111111</v>
       </c>
     </row>
@@ -1033,7 +1048,7 @@
       <c r="I11" s="1">
         <v>0</v>
       </c>
-      <c r="J11" s="1">
+      <c r="J11" s="5">
         <v>0.12847222222222224</v>
       </c>
       <c r="K11" s="1">
@@ -1042,16 +1057,16 @@
       <c r="L11" s="2">
         <v>0.91736111111111107</v>
       </c>
-      <c r="M11" s="2">
+      <c r="M11" s="6">
         <v>1.7388888888888889</v>
       </c>
       <c r="N11" s="2">
         <v>1.9152777777777779</v>
       </c>
-      <c r="O11" s="2">
+      <c r="O11" s="6">
         <v>1.9166666666666667</v>
       </c>
-      <c r="P11" s="2">
+      <c r="P11" s="6">
         <v>1.9993055555555557</v>
       </c>
     </row>
@@ -1080,7 +1095,7 @@
       <c r="I12" s="1">
         <v>0</v>
       </c>
-      <c r="J12" s="1">
+      <c r="J12" s="5">
         <v>0.11666666666666665</v>
       </c>
       <c r="K12" s="1">
@@ -1089,13 +1104,13 @@
       <c r="L12" s="2">
         <v>1.2527777777777778</v>
       </c>
-      <c r="M12" s="2">
+      <c r="M12" s="6">
         <v>1.7222222222222223</v>
       </c>
       <c r="N12" s="2">
         <v>1.8993055555555556</v>
       </c>
-      <c r="O12" s="2">
+      <c r="O12" s="6">
         <v>1.8993055555555556</v>
       </c>
     </row>
@@ -1124,7 +1139,7 @@
       <c r="I13" s="1">
         <v>4.1666666666666664E-2</v>
       </c>
-      <c r="J13" s="1">
+      <c r="J13" s="5">
         <v>0.12847222222222224</v>
       </c>
       <c r="K13" s="1">
@@ -1133,13 +1148,13 @@
       <c r="L13" s="2">
         <v>1.1805555555555556</v>
       </c>
-      <c r="M13" s="2">
+      <c r="M13" s="6">
         <v>1.8041666666666665</v>
       </c>
       <c r="N13" s="2">
         <v>1.95</v>
       </c>
-      <c r="O13" s="2">
+      <c r="O13" s="6">
         <v>1.95</v>
       </c>
     </row>
@@ -1165,7 +1180,7 @@
       <c r="I14" s="1">
         <v>0</v>
       </c>
-      <c r="J14" s="1">
+      <c r="J14" s="5">
         <v>0.12847222222222224</v>
       </c>
       <c r="K14" s="1">
@@ -1174,13 +1189,13 @@
       <c r="L14" s="2">
         <v>1.3472222222222223</v>
       </c>
-      <c r="M14" s="2">
+      <c r="M14" s="6">
         <v>1.7562499999999999</v>
       </c>
       <c r="N14" s="2">
         <v>1.9284722222222221</v>
       </c>
-      <c r="O14" s="2">
+      <c r="O14" s="6">
         <v>1.9291666666666665</v>
       </c>
     </row>
@@ -1207,7 +1222,7 @@
         <v>119</v>
       </c>
       <c r="I15" s="1"/>
-      <c r="J15" s="1"/>
+      <c r="J15" s="5"/>
       <c r="K15" s="1"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Remove highlighting from test spreadsheet.
</commit_message>
<xml_diff>
--- a/spec/fixtures/files/baddata2015test.xlsx
+++ b/spec/fixtures/files/baddata2015test.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27610"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27715"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -246,18 +246,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -272,15 +266,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="46" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="20" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="46" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="15" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="46" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -564,666 +555,664 @@
   <dimension ref="A1:P15"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="M6" sqref="M6"/>
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="10" max="10" width="10.83203125" style="4"/>
-    <col min="13" max="13" width="10.83203125" style="4"/>
-    <col min="15" max="16" width="10.83203125" style="4"/>
+    <col min="1" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="J1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="K1" t="s">
+      <c r="K1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="L1" t="s">
+      <c r="L1" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="M1" s="4" t="s">
+      <c r="M1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="N1" t="s">
+      <c r="N1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="O1" s="4" t="s">
+      <c r="O1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="P1" s="4" t="s">
+      <c r="P1" s="1" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+      <c r="A2" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="I2">
+      <c r="I2" s="1">
         <v>0</v>
       </c>
-      <c r="J2" s="4">
+      <c r="J2" s="1">
         <v>6.5</v>
       </c>
-      <c r="K2">
+      <c r="K2" s="1">
         <v>6.5</v>
       </c>
-      <c r="L2">
+      <c r="L2" s="1">
         <v>33</v>
       </c>
-      <c r="M2" s="4">
+      <c r="M2" s="1">
         <v>40</v>
       </c>
-      <c r="N2">
+      <c r="N2" s="1">
         <v>46.6</v>
       </c>
-      <c r="O2" s="4">
+      <c r="O2" s="1">
         <v>46.6</v>
       </c>
-      <c r="P2" s="4">
+      <c r="P2" s="1">
         <v>51.3</v>
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+      <c r="A3" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="F3">
+      <c r="F3" s="1">
         <v>28</v>
       </c>
-      <c r="G3" s="3">
+      <c r="G3" s="2">
         <v>31809</v>
       </c>
-      <c r="H3">
+      <c r="H3" s="1">
         <v>1</v>
       </c>
-      <c r="I3" s="1">
+      <c r="I3" s="3">
         <v>0</v>
       </c>
-      <c r="J3" s="5">
+      <c r="J3" s="3">
         <v>7.8472222222222221E-2</v>
       </c>
-      <c r="K3" s="1">
+      <c r="K3" s="3">
         <v>7.8472222222222221E-2</v>
       </c>
-      <c r="L3" s="1">
+      <c r="L3" s="3">
         <v>0.5625</v>
       </c>
-      <c r="M3" s="5">
+      <c r="M3" s="3">
         <v>0.8652777777777777</v>
       </c>
-      <c r="N3" s="1">
+      <c r="N3" s="3">
         <v>0.93125000000000002</v>
       </c>
-      <c r="O3" s="5">
+      <c r="O3" s="3">
         <v>0.93125000000000002</v>
       </c>
-      <c r="P3" s="5">
+      <c r="P3" s="3">
         <v>0.97777777777777775</v>
       </c>
     </row>
-    <row r="4" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="4" t="s">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="D4" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="E4" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="F4" s="4">
+      <c r="F4" s="1">
         <v>32</v>
       </c>
-      <c r="G4" s="7">
+      <c r="G4" s="2">
         <v>30390</v>
       </c>
-      <c r="H4" s="4">
+      <c r="H4" s="1">
         <v>128</v>
       </c>
-      <c r="I4" s="5">
+      <c r="I4" s="3">
         <v>0</v>
       </c>
-      <c r="J4" s="5">
+      <c r="J4" s="3">
         <v>8.4027777777777771E-2</v>
       </c>
-      <c r="K4" s="5">
+      <c r="K4" s="3">
         <v>8.4027777777777771E-2</v>
       </c>
-      <c r="L4" s="5">
+      <c r="L4" s="3">
         <v>0.58402777777777781</v>
       </c>
-      <c r="M4" s="5">
+      <c r="M4" s="3">
         <v>0.94791666666666663</v>
       </c>
-      <c r="N4" s="6">
+      <c r="N4" s="4">
         <v>0.84861111111111109</v>
       </c>
-      <c r="O4" s="6">
+      <c r="O4" s="4">
         <v>0.84861111111111109</v>
       </c>
-      <c r="P4" s="6">
+      <c r="P4" s="4">
         <v>1.0729166666666667</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+      <c r="A5" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E5" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="F5">
+      <c r="F5" s="1">
         <v>36</v>
       </c>
-      <c r="H5">
+      <c r="H5" s="1">
         <v>2</v>
       </c>
-      <c r="I5" s="1">
+      <c r="I5" s="3">
         <v>0</v>
       </c>
-      <c r="J5" s="5">
+      <c r="J5" s="3">
         <v>7.8472222222222221E-2</v>
       </c>
-      <c r="K5" s="1"/>
-      <c r="L5" s="1"/>
-      <c r="M5" s="5">
+      <c r="K5" s="3"/>
+      <c r="L5" s="3"/>
+      <c r="M5" s="3">
         <v>0.97361111111111109</v>
       </c>
-      <c r="N5" s="2">
+      <c r="N5" s="4">
         <v>1.0631944444444443</v>
       </c>
-      <c r="O5" s="6">
+      <c r="O5" s="4">
         <v>1.0638888888888889</v>
       </c>
-      <c r="P5" s="6">
+      <c r="P5" s="4">
         <v>1.117361111111111</v>
       </c>
     </row>
-    <row r="6" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="4" t="s">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="C6" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D6" s="4" t="s">
+      <c r="D6" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="E6" s="4" t="s">
+      <c r="E6" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="F6" s="4">
+      <c r="F6" s="1">
         <v>25</v>
       </c>
-      <c r="H6" s="4">
+      <c r="H6" s="1">
         <v>143</v>
       </c>
-      <c r="I6" s="5">
+      <c r="I6" s="3">
         <v>0</v>
       </c>
-      <c r="J6" s="5">
+      <c r="J6" s="3">
         <v>9.0277777777777776E-2</v>
       </c>
-      <c r="K6" s="5">
+      <c r="K6" s="3">
         <v>8.4027777777777771E-2</v>
       </c>
-      <c r="L6" s="5">
+      <c r="L6" s="3">
         <v>0.59722222222222221</v>
       </c>
-      <c r="M6" s="5">
+      <c r="M6" s="3">
         <v>0.98541666666666661</v>
       </c>
-      <c r="N6" s="6">
+      <c r="N6" s="4">
         <v>1.0763888888888888</v>
       </c>
-      <c r="O6" s="6">
+      <c r="O6" s="4">
         <v>1.0770833333333334</v>
       </c>
-      <c r="P6" s="6">
+      <c r="P6" s="4">
         <v>1.1270833333333334</v>
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
+      <c r="A7" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="E7" t="s">
+      <c r="E7" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F7">
+      <c r="F7" s="1">
         <v>51</v>
       </c>
-      <c r="H7">
+      <c r="H7" s="1">
         <v>30</v>
       </c>
-      <c r="I7" s="1">
+      <c r="I7" s="3">
         <v>2.0833333333333332E-2</v>
       </c>
-      <c r="J7" s="5">
+      <c r="J7" s="3">
         <v>0.11944444444444445</v>
       </c>
-      <c r="K7" s="1">
+      <c r="K7" s="3">
         <v>0.11944444444444445</v>
       </c>
-      <c r="L7" s="2">
+      <c r="L7" s="4">
         <v>0.84722222222222221</v>
       </c>
-      <c r="M7" s="6">
+      <c r="M7" s="4">
         <v>1.5625</v>
       </c>
-      <c r="N7" s="2">
+      <c r="N7" s="4">
         <v>1.7236111111111112</v>
       </c>
-      <c r="O7" s="6">
+      <c r="O7" s="4">
         <v>1.73125</v>
       </c>
-      <c r="P7" s="6">
+      <c r="P7" s="4">
         <v>1.8305555555555555</v>
       </c>
     </row>
-    <row r="8" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="4" t="s">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="B8" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="C8" s="4" t="s">
+      <c r="C8" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D8" s="4" t="s">
+      <c r="D8" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="E8" s="4" t="s">
+      <c r="E8" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="F8" s="4">
+      <c r="F8" s="1">
         <v>41</v>
       </c>
-      <c r="H8" s="4">
+      <c r="H8" s="1">
         <v>186</v>
       </c>
-      <c r="I8" s="5">
+      <c r="I8" s="3">
         <v>0</v>
       </c>
-      <c r="J8" s="5">
+      <c r="J8" s="3">
         <v>0.11805555555555557</v>
       </c>
-      <c r="K8" s="5">
+      <c r="K8" s="3">
         <v>0.11805555555555557</v>
       </c>
-      <c r="L8" s="6">
+      <c r="L8" s="4">
         <v>0.94027777777777777</v>
       </c>
-      <c r="M8" s="6">
+      <c r="M8" s="4">
         <v>1.5729166666666667</v>
       </c>
-      <c r="N8" s="6">
+      <c r="N8" s="4">
         <v>1.7229166666666667</v>
       </c>
-      <c r="O8" s="6">
+      <c r="O8" s="4">
         <v>1.7249999999999999</v>
       </c>
-      <c r="P8" s="6">
+      <c r="P8" s="4">
         <v>1.8319444444444446</v>
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
+      <c r="A9" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D9" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="E9" t="s">
+      <c r="E9" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="F9">
+      <c r="F9" s="1">
         <v>45</v>
       </c>
-      <c r="H9">
+      <c r="H9" s="1">
         <v>40</v>
       </c>
-      <c r="I9" s="1">
+      <c r="I9" s="3">
         <v>0</v>
       </c>
-      <c r="J9" s="5">
+      <c r="J9" s="3">
         <v>0.12916666666666668</v>
       </c>
-      <c r="K9" s="1">
+      <c r="K9" s="3">
         <v>0.12916666666666668</v>
       </c>
-      <c r="L9" s="2">
+      <c r="L9" s="4">
         <v>1.0347222222222221</v>
       </c>
-      <c r="M9" s="6">
+      <c r="M9" s="4">
         <v>1.6319444444444444</v>
       </c>
-      <c r="N9" s="2">
+      <c r="N9" s="4">
         <v>1.7944444444444445</v>
       </c>
-      <c r="O9" s="6">
+      <c r="O9" s="4">
         <v>1.7958333333333334</v>
       </c>
-      <c r="P9" s="6">
+      <c r="P9" s="4">
         <v>1.8965277777777778</v>
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
+      <c r="A10" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D10" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="E10" t="s">
+      <c r="E10" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="F10">
+      <c r="F10" s="1">
         <v>50</v>
       </c>
-      <c r="H10">
+      <c r="H10" s="1">
         <v>131</v>
       </c>
-      <c r="I10" s="1">
+      <c r="I10" s="3">
         <v>0</v>
       </c>
-      <c r="J10" s="5">
+      <c r="J10" s="3">
         <v>0.12847222222222224</v>
       </c>
-      <c r="K10" s="1">
+      <c r="K10" s="3">
         <v>0.12847222222222224</v>
       </c>
-      <c r="L10" s="2">
+      <c r="L10" s="4">
         <v>1.0374999999999999</v>
       </c>
-      <c r="M10" s="6"/>
-      <c r="N10" s="2">
+      <c r="M10" s="4"/>
+      <c r="N10" s="4">
         <v>1.8090277777777777</v>
       </c>
-      <c r="O10" s="6">
+      <c r="O10" s="4">
         <v>1.8138888888888889</v>
       </c>
-      <c r="P10" s="6">
+      <c r="P10" s="4">
         <v>1.9048611111111111</v>
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="B11" t="s">
+      <c r="B11" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D11" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="E11" t="s">
+      <c r="E11" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="F11">
+      <c r="F11" s="1">
         <v>41</v>
       </c>
-      <c r="H11">
+      <c r="H11" s="1">
         <v>122</v>
       </c>
-      <c r="I11" s="1">
+      <c r="I11" s="3">
         <v>0</v>
       </c>
-      <c r="J11" s="5">
+      <c r="J11" s="3">
         <v>0.12847222222222224</v>
       </c>
-      <c r="K11" s="1">
+      <c r="K11" s="3">
         <v>0.12847222222222224</v>
       </c>
-      <c r="L11" s="2">
+      <c r="L11" s="4">
         <v>0.91736111111111107</v>
       </c>
-      <c r="M11" s="6">
+      <c r="M11" s="4">
         <v>1.7388888888888889</v>
       </c>
-      <c r="N11" s="2">
+      <c r="N11" s="4">
         <v>1.9152777777777779</v>
       </c>
-      <c r="O11" s="6">
+      <c r="O11" s="4">
         <v>1.9166666666666667</v>
       </c>
-      <c r="P11" s="6">
+      <c r="P11" s="4">
         <v>1.9993055555555557</v>
       </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
+      <c r="A12" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C12" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D12" t="s">
+      <c r="D12" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="E12" t="s">
+      <c r="E12" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="F12">
+      <c r="F12" s="1">
         <v>62</v>
       </c>
-      <c r="H12">
+      <c r="H12" s="1">
         <v>49</v>
       </c>
-      <c r="I12" s="1">
+      <c r="I12" s="3">
         <v>0</v>
       </c>
-      <c r="J12" s="5">
+      <c r="J12" s="3">
         <v>0.11666666666666665</v>
       </c>
-      <c r="K12" s="1">
+      <c r="K12" s="3">
         <v>0.11666666666666665</v>
       </c>
-      <c r="L12" s="2">
+      <c r="L12" s="4">
         <v>1.2527777777777778</v>
       </c>
-      <c r="M12" s="6">
+      <c r="M12" s="4">
         <v>1.7222222222222223</v>
       </c>
-      <c r="N12" s="2">
+      <c r="N12" s="4">
         <v>1.8993055555555556</v>
       </c>
-      <c r="O12" s="6">
+      <c r="O12" s="4">
         <v>1.8993055555555556</v>
       </c>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
+      <c r="A13" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C13" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="D13" t="s">
+      <c r="D13" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E13" t="s">
+      <c r="E13" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="F13">
+      <c r="F13" s="1">
         <v>0</v>
       </c>
-      <c r="H13">
+      <c r="H13" s="1">
         <v>135</v>
       </c>
-      <c r="I13" s="1">
+      <c r="I13" s="3">
         <v>4.1666666666666664E-2</v>
       </c>
-      <c r="J13" s="5">
+      <c r="J13" s="3">
         <v>0.12847222222222224</v>
       </c>
-      <c r="K13" s="1">
+      <c r="K13" s="3">
         <v>0.12847222222222224</v>
       </c>
-      <c r="L13" s="2">
+      <c r="L13" s="4">
         <v>1.1805555555555556</v>
       </c>
-      <c r="M13" s="6">
+      <c r="M13" s="4">
         <v>1.8041666666666665</v>
       </c>
-      <c r="N13" s="2">
+      <c r="N13" s="4">
         <v>1.95</v>
       </c>
-      <c r="O13" s="6">
+      <c r="O13" s="4">
         <v>1.95</v>
       </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
+      <c r="A14" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C14" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D14" t="s">
+      <c r="D14" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="E14" t="s">
+      <c r="E14" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="H14">
+      <c r="H14" s="1">
         <v>32</v>
       </c>
-      <c r="I14" s="1">
+      <c r="I14" s="3">
         <v>0</v>
       </c>
-      <c r="J14" s="5">
+      <c r="J14" s="3">
         <v>0.12847222222222224</v>
       </c>
-      <c r="K14" s="1">
+      <c r="K14" s="3">
         <v>0.12847222222222224</v>
       </c>
-      <c r="L14" s="2">
+      <c r="L14" s="4">
         <v>1.3472222222222223</v>
       </c>
-      <c r="M14" s="6">
+      <c r="M14" s="4">
         <v>1.7562499999999999</v>
       </c>
-      <c r="N14" s="2">
+      <c r="N14" s="4">
         <v>1.9284722222222221</v>
       </c>
-      <c r="O14" s="6">
+      <c r="O14" s="4">
         <v>1.9291666666666665</v>
       </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
+      <c r="A15" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C15" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D15" t="s">
+      <c r="D15" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="E15" t="s">
+      <c r="E15" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="F15">
+      <c r="F15" s="1">
         <v>49</v>
       </c>
-      <c r="H15">
+      <c r="H15" s="1">
         <v>119</v>
       </c>
-      <c r="I15" s="1"/>
-      <c r="J15" s="5"/>
-      <c r="K15" s="1"/>
+      <c r="I15" s="3"/>
+      <c r="J15" s="3"/>
+      <c r="K15" s="3"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>

<commit_message>
Silence Auditable warnings in test environment; remove Auditable warning for Auditable#update_updated_by; Add Auditable spec; define factory for Race; define base factory for SplitTime; update baddata2015test.xlsx and EffortImporter tests to test for effort without start_split but with times at later splits; add Auditable tests to Course, Effort, Event, Location, Participant, Race, Split, and SplitTime.
</commit_message>
<xml_diff>
--- a/spec/fixtures/files/baddata2015test.xlsx
+++ b/spec/fixtures/files/baddata2015test.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27715"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27907"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="67">
   <si>
     <t>first_name</t>
   </si>
@@ -225,6 +225,12 @@
   </si>
   <si>
     <t>birthdate</t>
+  </si>
+  <si>
+    <t>StartSplit</t>
+  </si>
+  <si>
+    <t>NY</t>
   </si>
 </sst>
 </file>
@@ -552,10 +558,10 @@
   <sheetPr enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:P15"/>
+  <dimension ref="A1:P16"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+      <selection activeCell="L16" sqref="L16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1214,6 +1220,29 @@
       <c r="J15" s="3"/>
       <c r="K15" s="3"/>
     </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A16" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="H16" s="1">
+        <v>11</v>
+      </c>
+      <c r="J16" s="3">
+        <v>0.14583333333333334</v>
+      </c>
+      <c r="K16" s="3">
+        <v>0.14930555555555555</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Update tests to handle required home_time_zone field.
</commit_message>
<xml_diff>
--- a/spec/fixtures/files/baddata2015test.xlsx
+++ b/spec/fixtures/files/baddata2015test.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27907"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28209"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -561,7 +561,7 @@
   <dimension ref="A1:P16"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="L16" sqref="L16"/>
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Update baddata2015test spreadsheet file; update EffortImporter spec.
</commit_message>
<xml_diff>
--- a/spec/fixtures/files/baddata2015test.xlsx
+++ b/spec/fixtures/files/baddata2015test.xlsx
@@ -237,6 +237,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="[h]:mm:ss;@"/>
+  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -272,12 +275,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="46" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -561,7 +567,7 @@
   <dimension ref="A1:P16"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+      <selection activeCell="N6" sqref="N6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -627,25 +633,25 @@
         <v>0</v>
       </c>
       <c r="J2" s="1">
-        <v>6.5</v>
+        <v>10</v>
       </c>
       <c r="K2" s="1">
-        <v>6.5</v>
-      </c>
-      <c r="L2" s="1">
-        <v>33</v>
+        <v>10</v>
+      </c>
+      <c r="L2" s="5">
+        <v>70</v>
       </c>
       <c r="M2" s="1">
-        <v>40</v>
+        <v>100</v>
       </c>
       <c r="N2" s="1">
-        <v>46.6</v>
+        <v>120</v>
       </c>
       <c r="O2" s="1">
-        <v>46.6</v>
+        <v>120</v>
       </c>
       <c r="P2" s="1">
-        <v>51.3</v>
+        <v>140</v>
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.2">
@@ -677,25 +683,25 @@
         <v>0</v>
       </c>
       <c r="J3" s="3">
-        <v>7.8472222222222221E-2</v>
+        <v>8.3333333333333329E-2</v>
       </c>
       <c r="K3" s="3">
-        <v>7.8472222222222221E-2</v>
+        <v>8.4027777777777771E-2</v>
       </c>
       <c r="L3" s="3">
-        <v>0.5625</v>
+        <v>0.58680555555555558</v>
       </c>
       <c r="M3" s="3">
-        <v>0.8652777777777777</v>
-      </c>
-      <c r="N3" s="3">
-        <v>0.93125000000000002</v>
-      </c>
-      <c r="O3" s="3">
-        <v>0.93125000000000002</v>
-      </c>
-      <c r="P3" s="3">
-        <v>0.97777777777777775</v>
+        <v>0.84375</v>
+      </c>
+      <c r="N3" s="6">
+        <v>1.0138888888888888</v>
+      </c>
+      <c r="O3" s="6">
+        <v>1.0208333333333333</v>
+      </c>
+      <c r="P3" s="6">
+        <v>1.1875</v>
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.2">
@@ -733,19 +739,19 @@
         <v>8.4027777777777771E-2</v>
       </c>
       <c r="L4" s="3">
-        <v>0.58402777777777781</v>
+        <v>0.5854166666666667</v>
       </c>
       <c r="M4" s="3">
-        <v>0.94791666666666663</v>
-      </c>
-      <c r="N4" s="4">
-        <v>0.84861111111111109</v>
-      </c>
-      <c r="O4" s="4">
-        <v>0.84861111111111109</v>
-      </c>
-      <c r="P4" s="4">
-        <v>1.0729166666666667</v>
+        <v>0.88958333333333339</v>
+      </c>
+      <c r="N4" s="6">
+        <v>1.0069444444444444</v>
+      </c>
+      <c r="O4" s="6">
+        <v>1.0104166666666667</v>
+      </c>
+      <c r="P4" s="6">
+        <v>1.1888888888888889</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.2">
@@ -774,21 +780,21 @@
         <v>0</v>
       </c>
       <c r="J5" s="3">
-        <v>7.8472222222222221E-2</v>
+        <v>8.6111111111111124E-2</v>
       </c>
       <c r="K5" s="3"/>
       <c r="L5" s="3"/>
       <c r="M5" s="3">
         <v>0.97361111111111109</v>
       </c>
-      <c r="N5" s="4">
+      <c r="N5" s="6">
         <v>1.0631944444444443</v>
       </c>
-      <c r="O5" s="4">
+      <c r="O5" s="6">
         <v>1.0638888888888889</v>
       </c>
-      <c r="P5" s="4">
-        <v>1.117361111111111</v>
+      <c r="P5" s="6">
+        <v>1.2092824074074073</v>
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.2">
@@ -820,22 +826,22 @@
         <v>9.0277777777777776E-2</v>
       </c>
       <c r="K6" s="3">
-        <v>8.4027777777777771E-2</v>
+        <v>9.0277777777777776E-2</v>
       </c>
       <c r="L6" s="3">
         <v>0.59722222222222221</v>
       </c>
       <c r="M6" s="3">
-        <v>0.98541666666666661</v>
-      </c>
-      <c r="N6" s="4">
+        <v>0.68055555555555547</v>
+      </c>
+      <c r="N6" s="6">
         <v>1.0763888888888888</v>
       </c>
-      <c r="O6" s="4">
+      <c r="O6" s="6">
         <v>1.0770833333333334</v>
       </c>
-      <c r="P6" s="4">
-        <v>1.1270833333333334</v>
+      <c r="P6" s="6">
+        <v>1.2099884259259259</v>
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.2">
@@ -873,16 +879,16 @@
         <v>0.84722222222222221</v>
       </c>
       <c r="M7" s="4">
-        <v>1.5625</v>
-      </c>
-      <c r="N7" s="4">
+        <v>1.4375</v>
+      </c>
+      <c r="N7" s="6">
         <v>1.7236111111111112</v>
       </c>
-      <c r="O7" s="4">
+      <c r="O7" s="6">
         <v>1.73125</v>
       </c>
-      <c r="P7" s="4">
-        <v>1.8305555555555555</v>
+      <c r="P7" s="6">
+        <v>1.9555555555555555</v>
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.2">
@@ -914,7 +920,7 @@
         <v>0.11805555555555557</v>
       </c>
       <c r="K8" s="3">
-        <v>0.11805555555555557</v>
+        <v>8.6805555555555566E-2</v>
       </c>
       <c r="L8" s="4">
         <v>0.94027777777777777</v>
@@ -922,14 +928,14 @@
       <c r="M8" s="4">
         <v>1.5729166666666667</v>
       </c>
-      <c r="N8" s="4">
-        <v>1.7229166666666667</v>
-      </c>
-      <c r="O8" s="4">
-        <v>1.7249999999999999</v>
-      </c>
-      <c r="P8" s="4">
-        <v>1.8319444444444446</v>
+      <c r="N8" s="6">
+        <v>1.8479166666666667</v>
+      </c>
+      <c r="O8" s="6">
+        <v>1.8499999999999999</v>
+      </c>
+      <c r="P8" s="7">
+        <v>2.1180555555555558</v>
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.2">
@@ -969,14 +975,14 @@
       <c r="M9" s="4">
         <v>1.6319444444444444</v>
       </c>
-      <c r="N9" s="4">
-        <v>1.7944444444444445</v>
-      </c>
-      <c r="O9" s="4">
-        <v>1.7958333333333334</v>
-      </c>
-      <c r="P9" s="4">
-        <v>1.8965277777777778</v>
+      <c r="N9" s="6">
+        <v>1.9194444444444445</v>
+      </c>
+      <c r="O9" s="6">
+        <v>1.9513888888888891</v>
+      </c>
+      <c r="P9" s="6">
+        <v>2.1829050925925926</v>
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.2">
@@ -1011,14 +1017,14 @@
         <v>1.0374999999999999</v>
       </c>
       <c r="M10" s="4"/>
-      <c r="N10" s="4">
-        <v>1.8090277777777777</v>
-      </c>
-      <c r="O10" s="4">
-        <v>1.8138888888888889</v>
-      </c>
-      <c r="P10" s="4">
-        <v>1.9048611111111111</v>
+      <c r="N10" s="6">
+        <v>1.9909722222222221</v>
+      </c>
+      <c r="O10" s="6">
+        <v>1.9916666666666665</v>
+      </c>
+      <c r="P10" s="6">
+        <v>2.2168055555555557</v>
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.2">
@@ -1050,19 +1056,19 @@
         <v>0.12847222222222224</v>
       </c>
       <c r="L11" s="4">
-        <v>0.91736111111111107</v>
+        <v>1.0798611111111112</v>
       </c>
       <c r="M11" s="4">
         <v>1.7388888888888889</v>
       </c>
-      <c r="N11" s="4">
-        <v>1.9152777777777779</v>
-      </c>
-      <c r="O11" s="4">
-        <v>1.9166666666666667</v>
-      </c>
-      <c r="P11" s="4">
-        <v>1.9993055555555557</v>
+      <c r="N11" s="6">
+        <v>2</v>
+      </c>
+      <c r="O11" s="6">
+        <v>2.0000115740740738</v>
+      </c>
+      <c r="P11" s="6">
+        <v>2.2457523148148151</v>
       </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.2">
@@ -1097,17 +1103,18 @@
         <v>0.11666666666666665</v>
       </c>
       <c r="L12" s="4">
-        <v>1.2527777777777778</v>
+        <v>1.0027777777777778</v>
       </c>
       <c r="M12" s="4">
         <v>1.7222222222222223</v>
       </c>
-      <c r="N12" s="4">
-        <v>1.8993055555555556</v>
-      </c>
-      <c r="O12" s="4">
-        <v>1.8993055555555556</v>
-      </c>
+      <c r="N12" s="7">
+        <v>1.9979166666666668</v>
+      </c>
+      <c r="O12" s="6">
+        <v>1.9986111111111111</v>
+      </c>
+      <c r="P12" s="6"/>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
@@ -1146,12 +1153,13 @@
       <c r="M13" s="4">
         <v>1.8041666666666665</v>
       </c>
-      <c r="N13" s="4">
-        <v>1.95</v>
-      </c>
-      <c r="O13" s="4">
-        <v>1.95</v>
-      </c>
+      <c r="N13" s="6">
+        <v>2.0833449074074073</v>
+      </c>
+      <c r="O13" s="6">
+        <v>2.0861226851851851</v>
+      </c>
+      <c r="P13" s="6"/>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
@@ -1187,12 +1195,11 @@
       <c r="M14" s="4">
         <v>1.7562499999999999</v>
       </c>
-      <c r="N14" s="4">
+      <c r="N14" s="6">
         <v>1.9284722222222221</v>
       </c>
-      <c r="O14" s="4">
-        <v>1.9291666666666665</v>
-      </c>
+      <c r="O14" s="6"/>
+      <c r="P14" s="6"/>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">

</xml_diff>